<commit_message>
Luyện tập vòng lặp 02
</commit_message>
<xml_diff>
--- a/TaiLieuCodegym/_[A0321I1] TKB Bootcamp Preparation.xlsx
+++ b/TaiLieuCodegym/_[A0321I1] TKB Bootcamp Preparation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\A0321I1-MinhKhoa\TaiLieuCodegym\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FADE46C9-6A68-434F-BA58-92F4E9B46104}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E18E20-30F0-4558-B71C-911E2C06B80A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="128">
   <si>
     <t>THỜI KHOÁ BIỂU</t>
   </si>
@@ -1015,7 +1015,7 @@
   <dimension ref="A1:Y1001"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1874,9 +1874,8 @@
       <c r="E24" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="F24" s="31" t="str">
-        <f t="shared" ref="F23:F25" si="1">IF(C24="Th 6","Retros","")</f>
-        <v/>
+      <c r="F24" s="31" t="s">
+        <v>127</v>
       </c>
       <c r="G24" s="32"/>
       <c r="H24" s="21"/>
@@ -1917,7 +1916,7 @@
         <v>59</v>
       </c>
       <c r="F25" s="31" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="F24:F25" si="1">IF(C25="Th 6","Retros","")</f>
         <v/>
       </c>
       <c r="G25" s="32"/>

</xml_diff>

<commit_message>
bài tập mảng 2
</commit_message>
<xml_diff>
--- a/TaiLieuCodegym/_[A0321I1] TKB Bootcamp Preparation.xlsx
+++ b/TaiLieuCodegym/_[A0321I1] TKB Bootcamp Preparation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\A0321I1-MinhKhoa\TaiLieuCodegym\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E18E20-30F0-4558-B71C-911E2C06B80A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A54ED264-BC67-4094-BC26-0F9BB0FBC8AB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="128">
   <si>
     <t>THỜI KHOÁ BIỂU</t>
   </si>
@@ -1915,9 +1915,8 @@
       <c r="E25" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="F25" s="31" t="str">
-        <f t="shared" ref="F24:F25" si="1">IF(C25="Th 6","Retros","")</f>
-        <v/>
+      <c r="F25" s="31" t="s">
+        <v>127</v>
       </c>
       <c r="G25" s="32"/>
       <c r="H25" s="21"/>
@@ -2040,7 +2039,7 @@
         <v>70</v>
       </c>
       <c r="F28" s="31" t="str">
-        <f t="shared" ref="F28:F39" si="2">IF(C28="Th 6","Retros","")</f>
+        <f t="shared" ref="F28:F39" si="1">IF(C28="Th 6","Retros","")</f>
         <v/>
       </c>
       <c r="G28" s="32"/>
@@ -2082,7 +2081,7 @@
         <v>73</v>
       </c>
       <c r="F29" s="31" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G29" s="32"/>
@@ -2124,7 +2123,7 @@
         <v>76</v>
       </c>
       <c r="F30" s="31" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G30" s="32"/>
@@ -2166,7 +2165,7 @@
         <v>78</v>
       </c>
       <c r="F31" s="31" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G31" s="32"/>
@@ -2208,7 +2207,7 @@
         <v>80</v>
       </c>
       <c r="F32" s="31" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G32" s="32"/>
@@ -2250,7 +2249,7 @@
         <v>83</v>
       </c>
       <c r="F33" s="31" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G33" s="32"/>
@@ -2292,7 +2291,7 @@
         <v>86</v>
       </c>
       <c r="F34" s="31" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G34" s="32"/>
@@ -2334,7 +2333,7 @@
         <v>89</v>
       </c>
       <c r="F35" s="31" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G35" s="32"/>
@@ -2376,7 +2375,7 @@
         <v>92</v>
       </c>
       <c r="F36" s="31" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G36" s="32"/>
@@ -2418,7 +2417,7 @@
         <v>95</v>
       </c>
       <c r="F37" s="31" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G37" s="32"/>
@@ -2460,7 +2459,7 @@
         <v>98</v>
       </c>
       <c r="F38" s="31" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G38" s="32"/>
@@ -2502,7 +2501,7 @@
         <v>100</v>
       </c>
       <c r="F39" s="31" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G39" s="32"/>

</xml_diff>

<commit_message>
up product Management Applications
</commit_message>
<xml_diff>
--- a/TaiLieuCodegym/_[A0321I1] TKB Bootcamp Preparation.xlsx
+++ b/TaiLieuCodegym/_[A0321I1] TKB Bootcamp Preparation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\A0321I1-MinhKhoa\TaiLieuCodegym\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A54ED264-BC67-4094-BC26-0F9BB0FBC8AB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92CFD284-2E18-4C38-9E87-9CA0485A1F94}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="129">
   <si>
     <t>THỜI KHOÁ BIỂU</t>
   </si>
@@ -214,9 +214,6 @@
     <t>BP.T12</t>
   </si>
   <si>
-    <t>Seminar Technical</t>
-  </si>
-  <si>
     <t>Buổi 15</t>
   </si>
   <si>
@@ -407,6 +404,12 @@
   </si>
   <si>
     <t>r</t>
+  </si>
+  <si>
+    <t>Seminar Technical r</t>
+  </si>
+  <si>
+    <t>Retros CAH r</t>
   </si>
 </sst>
 </file>
@@ -1014,8 +1017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1426,7 +1429,7 @@
         <v>26</v>
       </c>
       <c r="F13" s="31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G13" s="32"/>
       <c r="H13" s="21"/>
@@ -1467,7 +1470,7 @@
         <v>29</v>
       </c>
       <c r="F14" s="31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G14" s="32"/>
       <c r="H14" s="21"/>
@@ -1508,7 +1511,7 @@
         <v>32</v>
       </c>
       <c r="F15" s="31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G15" s="32"/>
       <c r="H15" s="21"/>
@@ -1549,7 +1552,7 @@
         <v>35</v>
       </c>
       <c r="F16" s="31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G16" s="32"/>
       <c r="H16" s="21"/>
@@ -1590,7 +1593,7 @@
         <v>38</v>
       </c>
       <c r="F17" s="31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G17" s="32"/>
       <c r="H17" s="21"/>
@@ -1631,7 +1634,7 @@
         <v>40</v>
       </c>
       <c r="F18" s="31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G18" s="32"/>
       <c r="H18" s="21"/>
@@ -1672,7 +1675,7 @@
         <v>42</v>
       </c>
       <c r="F19" s="31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G19" s="32"/>
       <c r="H19" s="21"/>
@@ -1713,7 +1716,7 @@
         <v>45</v>
       </c>
       <c r="F20" s="31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G20" s="32"/>
       <c r="H20" s="21"/>
@@ -1754,7 +1757,7 @@
         <v>48</v>
       </c>
       <c r="F21" s="31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G21" s="32"/>
       <c r="H21" s="21"/>
@@ -1793,7 +1796,7 @@
       </c>
       <c r="E22" s="49"/>
       <c r="F22" s="31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G22" s="32"/>
       <c r="H22" s="21"/>
@@ -1834,7 +1837,7 @@
         <v>53</v>
       </c>
       <c r="F23" s="31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G23" s="32"/>
       <c r="H23" s="21"/>
@@ -1875,7 +1878,7 @@
         <v>56</v>
       </c>
       <c r="F24" s="31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G24" s="32"/>
       <c r="H24" s="21"/>
@@ -1916,7 +1919,7 @@
         <v>59</v>
       </c>
       <c r="F25" s="31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G25" s="32"/>
       <c r="H25" s="21"/>
@@ -1957,7 +1960,7 @@
         <v>62</v>
       </c>
       <c r="F26" s="37" t="s">
-        <v>63</v>
+        <v>127</v>
       </c>
       <c r="G26" s="32"/>
       <c r="H26" s="21"/>
@@ -1981,7 +1984,7 @@
     </row>
     <row r="27" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B27" s="33">
         <f>WORKDAY(B26,2,'Holidays 2021,2020'!$B$2:$B$19)</f>
@@ -1992,13 +1995,13 @@
         <v>Mon</v>
       </c>
       <c r="D27" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="E27" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="E27" s="35" t="s">
-        <v>66</v>
-      </c>
       <c r="F27" s="31" t="s">
-        <v>67</v>
+        <v>128</v>
       </c>
       <c r="G27" s="32"/>
       <c r="H27" s="21"/>
@@ -2022,7 +2025,7 @@
     </row>
     <row r="28" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B28" s="33">
         <f>WORKDAY(B27,2,'Holidays 2021,2020'!$B$2:$B$19)</f>
@@ -2033,15 +2036,12 @@
         <v>Wed</v>
       </c>
       <c r="D28" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="E28" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="E28" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="F28" s="31" t="str">
-        <f t="shared" ref="F28:F39" si="1">IF(C28="Th 6","Retros","")</f>
-        <v/>
-      </c>
+      <c r="F28" s="31"/>
       <c r="G28" s="32"/>
       <c r="H28" s="21"/>
       <c r="I28" s="9"/>
@@ -2064,7 +2064,7 @@
     </row>
     <row r="29" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B29" s="33">
         <f>WORKDAY(B28,2,'Holidays 2021,2020'!$B$2:$B$19)</f>
@@ -2075,13 +2075,13 @@
         <v>Fri</v>
       </c>
       <c r="D29" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="E29" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="E29" s="35" t="s">
-        <v>73</v>
-      </c>
       <c r="F29" s="31" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="F28:F39" si="1">IF(C29="Th 6","Retros","")</f>
         <v/>
       </c>
       <c r="G29" s="32"/>
@@ -2106,7 +2106,7 @@
     </row>
     <row r="30" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B30" s="33">
         <f>WORKDAY(B29,1,'Holidays 2021,2020'!$B$2:$B$19)</f>
@@ -2117,10 +2117,10 @@
         <v>Mon</v>
       </c>
       <c r="D30" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="E30" s="35" t="s">
         <v>75</v>
-      </c>
-      <c r="E30" s="35" t="s">
-        <v>76</v>
       </c>
       <c r="F30" s="31" t="str">
         <f t="shared" si="1"/>
@@ -2148,7 +2148,7 @@
     </row>
     <row r="31" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B31" s="33">
         <f>WORKDAY(B30,2,'Holidays 2021,2020'!$B$2:$B$19)</f>
@@ -2159,10 +2159,10 @@
         <v>Wed</v>
       </c>
       <c r="D31" s="29" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E31" s="36" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F31" s="31" t="str">
         <f t="shared" si="1"/>
@@ -2190,7 +2190,7 @@
     </row>
     <row r="32" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B32" s="33">
         <f>WORKDAY(B31,2,'Holidays 2021,2020'!$B$2:$B$19)</f>
@@ -2201,10 +2201,10 @@
         <v>Fri</v>
       </c>
       <c r="D32" s="29" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E32" s="35" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F32" s="31" t="str">
         <f t="shared" si="1"/>
@@ -2232,7 +2232,7 @@
     </row>
     <row r="33" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B33" s="33">
         <f>WORKDAY(B32,1,'Holidays 2021,2020'!$B$2:$B$19)</f>
@@ -2243,10 +2243,10 @@
         <v>Mon</v>
       </c>
       <c r="D33" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="E33" s="35" t="s">
         <v>82</v>
-      </c>
-      <c r="E33" s="35" t="s">
-        <v>83</v>
       </c>
       <c r="F33" s="31" t="str">
         <f t="shared" si="1"/>
@@ -2274,7 +2274,7 @@
     </row>
     <row r="34" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B34" s="33">
         <f>WORKDAY(B33,2,'Holidays 2021,2020'!$B$2:$B$19)</f>
@@ -2285,10 +2285,10 @@
         <v>Wed</v>
       </c>
       <c r="D34" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="E34" s="35" t="s">
         <v>85</v>
-      </c>
-      <c r="E34" s="35" t="s">
-        <v>86</v>
       </c>
       <c r="F34" s="31" t="str">
         <f t="shared" si="1"/>
@@ -2316,7 +2316,7 @@
     </row>
     <row r="35" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B35" s="33">
         <f>WORKDAY(B34,2,'Holidays 2021,2020'!$B$2:$B$19)</f>
@@ -2327,10 +2327,10 @@
         <v>Fri</v>
       </c>
       <c r="D35" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="E35" s="35" t="s">
         <v>88</v>
-      </c>
-      <c r="E35" s="35" t="s">
-        <v>89</v>
       </c>
       <c r="F35" s="31" t="str">
         <f t="shared" si="1"/>
@@ -2358,7 +2358,7 @@
     </row>
     <row r="36" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B36" s="33">
         <f>WORKDAY(B35,1,'Holidays 2021,2020'!$B$2:$B$19)</f>
@@ -2369,10 +2369,10 @@
         <v>Mon</v>
       </c>
       <c r="D36" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="E36" s="36" t="s">
         <v>91</v>
-      </c>
-      <c r="E36" s="36" t="s">
-        <v>92</v>
       </c>
       <c r="F36" s="31" t="str">
         <f t="shared" si="1"/>
@@ -2400,7 +2400,7 @@
     </row>
     <row r="37" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B37" s="33">
         <f>WORKDAY(B36,2,'Holidays 2021,2020'!$B$2:$B$19)</f>
@@ -2411,10 +2411,10 @@
         <v>Wed</v>
       </c>
       <c r="D37" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="E37" s="35" t="s">
         <v>94</v>
-      </c>
-      <c r="E37" s="35" t="s">
-        <v>95</v>
       </c>
       <c r="F37" s="31" t="str">
         <f t="shared" si="1"/>
@@ -2442,7 +2442,7 @@
     </row>
     <row r="38" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B38" s="33">
         <f>WORKDAY(B37,2,'Holidays 2021,2020'!$B$2:$B$19)</f>
@@ -2453,10 +2453,10 @@
         <v>Fri</v>
       </c>
       <c r="D38" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="E38" s="35" t="s">
         <v>97</v>
-      </c>
-      <c r="E38" s="35" t="s">
-        <v>98</v>
       </c>
       <c r="F38" s="31" t="str">
         <f t="shared" si="1"/>
@@ -2484,7 +2484,7 @@
     </row>
     <row r="39" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A39" s="26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B39" s="33">
         <f>WORKDAY(B38,1,'Holidays 2021,2020'!$B$2:$B$19)</f>
@@ -2495,10 +2495,10 @@
         <v>Mon</v>
       </c>
       <c r="D39" s="29" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E39" s="29" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F39" s="31" t="str">
         <f t="shared" si="1"/>
@@ -2526,7 +2526,7 @@
     </row>
     <row r="40" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B40" s="33">
         <f>WORKDAY(B39,2,'Holidays 2021,2020'!$B$2:$B$19)</f>
@@ -2537,13 +2537,13 @@
         <v>Wed</v>
       </c>
       <c r="D40" s="38" t="s">
+        <v>101</v>
+      </c>
+      <c r="E40" s="38" t="s">
+        <v>101</v>
+      </c>
+      <c r="F40" s="39" t="s">
         <v>102</v>
-      </c>
-      <c r="E40" s="38" t="s">
-        <v>102</v>
-      </c>
-      <c r="F40" s="39" t="s">
-        <v>103</v>
       </c>
       <c r="G40" s="32"/>
       <c r="H40" s="21"/>
@@ -2567,7 +2567,7 @@
     </row>
     <row r="41" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="26" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B41" s="33">
         <f>WORKDAY(B40,2,'Holidays 2021,2020'!$B$2:$B$19)</f>
@@ -2578,13 +2578,13 @@
         <v>Fri</v>
       </c>
       <c r="D41" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="E41" s="41" t="s">
         <v>105</v>
       </c>
-      <c r="E41" s="41" t="s">
+      <c r="F41" s="42" t="s">
         <v>106</v>
-      </c>
-      <c r="F41" s="42" t="s">
-        <v>107</v>
       </c>
       <c r="G41" s="32"/>
       <c r="H41" s="21"/>
@@ -2609,10 +2609,10 @@
     <row r="42" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="43"/>
       <c r="B42" s="44" t="s">
+        <v>107</v>
+      </c>
+      <c r="C42" s="8" t="s">
         <v>108</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>109</v>
       </c>
       <c r="D42" s="8"/>
       <c r="E42" s="8"/>
@@ -2640,10 +2640,10 @@
     <row r="43" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="8"/>
       <c r="B43" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C43" s="8" t="s">
         <v>110</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>111</v>
       </c>
       <c r="D43" s="8"/>
       <c r="E43" s="8"/>
@@ -2671,10 +2671,10 @@
     <row r="44" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="8"/>
       <c r="B44" s="45" t="s">
+        <v>111</v>
+      </c>
+      <c r="C44" s="8" t="s">
         <v>112</v>
-      </c>
-      <c r="C44" s="8" t="s">
-        <v>113</v>
       </c>
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
@@ -2702,10 +2702,10 @@
     <row r="45" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="8"/>
       <c r="B45" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C45" s="8" t="s">
         <v>114</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>115</v>
       </c>
       <c r="D45" s="8"/>
       <c r="E45" s="8"/>
@@ -2733,10 +2733,10 @@
     <row r="46" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="8"/>
       <c r="B46" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D46" s="8"/>
       <c r="E46" s="8"/>
@@ -8944,13 +8944,13 @@
   <sheetData>
     <row r="1" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -8981,7 +8981,7 @@
         <v>44197</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -9012,7 +9012,7 @@
         <v>44235</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -9043,7 +9043,7 @@
         <v>44236</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -9074,7 +9074,7 @@
         <v>43850</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -9105,7 +9105,7 @@
         <v>44237</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -9136,7 +9136,7 @@
         <v>44238</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -9167,7 +9167,7 @@
         <v>44239</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -9198,7 +9198,7 @@
         <v>44240</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -9229,7 +9229,7 @@
         <v>44241</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -9260,7 +9260,7 @@
         <v>44242</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -9291,7 +9291,7 @@
         <v>44243</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -9322,7 +9322,7 @@
         <v>44244</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -9353,7 +9353,7 @@
         <v>44245</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -9384,7 +9384,7 @@
         <v>44246</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -9415,7 +9415,7 @@
         <v>44307</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -9446,7 +9446,7 @@
         <v>44316</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -9477,7 +9477,7 @@
         <v>44317</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -9508,7 +9508,7 @@
         <v>44441</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>

</xml_diff>

<commit_message>
up thực hành bài 16 hướng đối tượng 1
</commit_message>
<xml_diff>
--- a/TaiLieuCodegym/_[A0321I1] TKB Bootcamp Preparation.xlsx
+++ b/TaiLieuCodegym/_[A0321I1] TKB Bootcamp Preparation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\A0321I1-MinhKhoa\TaiLieuCodegym\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92CFD284-2E18-4C38-9E87-9CA0485A1F94}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E44EC8-BE62-489A-84C6-19EA6F6DDDDB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="129">
   <si>
     <t>THỜI KHOÁ BIỂU</t>
   </si>
@@ -2041,7 +2041,9 @@
       <c r="E28" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="F28" s="31"/>
+      <c r="F28" s="31" t="s">
+        <v>126</v>
+      </c>
       <c r="G28" s="32"/>
       <c r="H28" s="21"/>
       <c r="I28" s="9"/>
@@ -2081,7 +2083,7 @@
         <v>72</v>
       </c>
       <c r="F29" s="31" t="str">
-        <f t="shared" ref="F28:F39" si="1">IF(C29="Th 6","Retros","")</f>
+        <f t="shared" ref="F29:F39" si="1">IF(C29="Th 6","Retros","")</f>
         <v/>
       </c>
       <c r="G29" s="32"/>

</xml_diff>

<commit_message>
up bài 16.Xây dựng lớp mô tả Temperature
</commit_message>
<xml_diff>
--- a/TaiLieuCodegym/_[A0321I1] TKB Bootcamp Preparation.xlsx
+++ b/TaiLieuCodegym/_[A0321I1] TKB Bootcamp Preparation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\A0321I1-MinhKhoa\TaiLieuCodegym\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E44EC8-BE62-489A-84C6-19EA6F6DDDDB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37302B11-2F7A-41CF-896F-42A17E6D0325}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="129">
   <si>
     <t>THỜI KHOÁ BIỂU</t>
   </si>
@@ -1018,7 +1018,7 @@
   <dimension ref="A1:Y1001"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2082,9 +2082,8 @@
       <c r="E29" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="F29" s="31" t="str">
-        <f t="shared" ref="F29:F39" si="1">IF(C29="Th 6","Retros","")</f>
-        <v/>
+      <c r="F29" s="31" t="s">
+        <v>126</v>
       </c>
       <c r="G29" s="32"/>
       <c r="H29" s="21"/>
@@ -2125,7 +2124,7 @@
         <v>75</v>
       </c>
       <c r="F30" s="31" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="F29:F39" si="1">IF(C30="Th 6","Retros","")</f>
         <v/>
       </c>
       <c r="G30" s="32"/>

</xml_diff>

<commit_message>
up bài thực hành bài 17
</commit_message>
<xml_diff>
--- a/TaiLieuCodegym/_[A0321I1] TKB Bootcamp Preparation.xlsx
+++ b/TaiLieuCodegym/_[A0321I1] TKB Bootcamp Preparation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\A0321I1-MinhKhoa\TaiLieuCodegym\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37302B11-2F7A-41CF-896F-42A17E6D0325}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA01D39-1208-4EC3-8722-9AE9445710B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="129">
   <si>
     <t>THỜI KHOÁ BIỂU</t>
   </si>
@@ -1018,7 +1018,7 @@
   <dimension ref="A1:Y1001"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2123,9 +2123,8 @@
       <c r="E30" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="F30" s="31" t="str">
-        <f t="shared" ref="F29:F39" si="1">IF(C30="Th 6","Retros","")</f>
-        <v/>
+      <c r="F30" s="31" t="s">
+        <v>126</v>
       </c>
       <c r="G30" s="32"/>
       <c r="H30" s="21"/>
@@ -2166,7 +2165,7 @@
         <v>77</v>
       </c>
       <c r="F31" s="31" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="F30:F39" si="1">IF(C31="Th 6","Retros","")</f>
         <v/>
       </c>
       <c r="G31" s="32"/>

</xml_diff>

<commit_message>
up bài tập 17. cờ ca rô
</commit_message>
<xml_diff>
--- a/TaiLieuCodegym/_[A0321I1] TKB Bootcamp Preparation.xlsx
+++ b/TaiLieuCodegym/_[A0321I1] TKB Bootcamp Preparation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\A0321I1-MinhKhoa\TaiLieuCodegym\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA01D39-1208-4EC3-8722-9AE9445710B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FD1A708-0DE1-41B5-83C9-66D4881C8303}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="129">
   <si>
     <t>THỜI KHOÁ BIỂU</t>
   </si>
@@ -1018,7 +1018,7 @@
   <dimension ref="A1:Y1001"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2164,9 +2164,8 @@
       <c r="E31" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="F31" s="31" t="str">
-        <f t="shared" ref="F30:F39" si="1">IF(C31="Th 6","Retros","")</f>
-        <v/>
+      <c r="F31" s="31" t="s">
+        <v>126</v>
       </c>
       <c r="G31" s="32"/>
       <c r="H31" s="21"/>
@@ -2207,7 +2206,7 @@
         <v>79</v>
       </c>
       <c r="F32" s="31" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="F31:F39" si="1">IF(C32="Th 6","Retros","")</f>
         <v/>
       </c>
       <c r="G32" s="32"/>

</xml_diff>

<commit_message>
up thuat toan 1
</commit_message>
<xml_diff>
--- a/TaiLieuCodegym/_[A0321I1] TKB Bootcamp Preparation.xlsx
+++ b/TaiLieuCodegym/_[A0321I1] TKB Bootcamp Preparation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\A0321I1-MinhKhoa\TaiLieuCodegym\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FD1A708-0DE1-41B5-83C9-66D4881C8303}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{512000DB-BD74-4C5F-80A9-D535CF6225A8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="129">
   <si>
     <t>THỜI KHOÁ BIỂU</t>
   </si>
@@ -2205,9 +2205,8 @@
       <c r="E32" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="F32" s="31" t="str">
-        <f t="shared" ref="F31:F39" si="1">IF(C32="Th 6","Retros","")</f>
-        <v/>
+      <c r="F32" s="31" t="s">
+        <v>126</v>
       </c>
       <c r="G32" s="32"/>
       <c r="H32" s="21"/>
@@ -2248,7 +2247,7 @@
         <v>82</v>
       </c>
       <c r="F33" s="31" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="F32:F39" si="1">IF(C33="Th 6","Retros","")</f>
         <v/>
       </c>
       <c r="G33" s="32"/>

</xml_diff>

<commit_message>
up case study requirements3 bai 1234
</commit_message>
<xml_diff>
--- a/TaiLieuCodegym/_[A0321I1] TKB Bootcamp Preparation.xlsx
+++ b/TaiLieuCodegym/_[A0321I1] TKB Bootcamp Preparation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\A0321I1-MinhKhoa\TaiLieuCodegym\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{512000DB-BD74-4C5F-80A9-D535CF6225A8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB803230-2C22-4E8B-8D4A-DF54097F0EE8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="129">
   <si>
     <t>THỜI KHOÁ BIỂU</t>
   </si>
@@ -1017,8 +1017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2246,9 +2246,8 @@
       <c r="E33" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="F33" s="31" t="str">
-        <f t="shared" ref="F32:F39" si="1">IF(C33="Th 6","Retros","")</f>
-        <v/>
+      <c r="F33" s="31" t="s">
+        <v>126</v>
       </c>
       <c r="G33" s="32"/>
       <c r="H33" s="21"/>
@@ -2288,9 +2287,8 @@
       <c r="E34" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="F34" s="31" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="F34" s="31" t="s">
+        <v>126</v>
       </c>
       <c r="G34" s="32"/>
       <c r="H34" s="21"/>
@@ -2331,7 +2329,7 @@
         <v>88</v>
       </c>
       <c r="F35" s="31" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="F33:F39" si="1">IF(C35="Th 6","Retros","")</f>
         <v/>
       </c>
       <c r="G35" s="32"/>

</xml_diff>

<commit_message>
up case study requirements6
</commit_message>
<xml_diff>
--- a/TaiLieuCodegym/_[A0321I1] TKB Bootcamp Preparation.xlsx
+++ b/TaiLieuCodegym/_[A0321I1] TKB Bootcamp Preparation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\A0321I1-MinhKhoa\TaiLieuCodegym\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB803230-2C22-4E8B-8D4A-DF54097F0EE8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E992504-C9D6-49EE-AB80-E5C3AC5FD0A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="129">
   <si>
     <t>THỜI KHOÁ BIỂU</t>
   </si>
@@ -1017,8 +1017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2328,9 +2328,8 @@
       <c r="E35" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="F35" s="31" t="str">
-        <f t="shared" ref="F33:F39" si="1">IF(C35="Th 6","Retros","")</f>
-        <v/>
+      <c r="F35" s="31" t="s">
+        <v>126</v>
       </c>
       <c r="G35" s="32"/>
       <c r="H35" s="21"/>
@@ -2370,9 +2369,8 @@
       <c r="E36" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="F36" s="31" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="F36" s="31" t="s">
+        <v>126</v>
       </c>
       <c r="G36" s="32"/>
       <c r="H36" s="21"/>
@@ -2413,7 +2411,7 @@
         <v>94</v>
       </c>
       <c r="F37" s="31" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="F36:F39" si="1">IF(C37="Th 6","Retros","")</f>
         <v/>
       </c>
       <c r="G37" s="32"/>

</xml_diff>

<commit_message>
up case study requirements7
</commit_message>
<xml_diff>
--- a/TaiLieuCodegym/_[A0321I1] TKB Bootcamp Preparation.xlsx
+++ b/TaiLieuCodegym/_[A0321I1] TKB Bootcamp Preparation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\A0321I1-MinhKhoa\TaiLieuCodegym\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E992504-C9D6-49EE-AB80-E5C3AC5FD0A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AFC69F6-E8C1-443B-8678-643E1637B07A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="129">
   <si>
     <t>THỜI KHOÁ BIỂU</t>
   </si>
@@ -1018,7 +1018,7 @@
   <dimension ref="A1:Y1001"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2410,9 +2410,8 @@
       <c r="E37" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="F37" s="31" t="str">
-        <f t="shared" ref="F36:F39" si="1">IF(C37="Th 6","Retros","")</f>
-        <v/>
+      <c r="F37" s="31" t="s">
+        <v>126</v>
       </c>
       <c r="G37" s="32"/>
       <c r="H37" s="21"/>
@@ -2452,9 +2451,8 @@
       <c r="E38" s="35" t="s">
         <v>97</v>
       </c>
-      <c r="F38" s="31" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="F38" s="31" t="s">
+        <v>126</v>
       </c>
       <c r="G38" s="32"/>
       <c r="H38" s="21"/>
@@ -2495,7 +2493,7 @@
         <v>99</v>
       </c>
       <c r="F39" s="31" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="F37:F39" si="1">IF(C39="Th 6","Retros","")</f>
         <v/>
       </c>
       <c r="G39" s="32"/>

</xml_diff>